<commit_message>
Crie função para fazer buscas no Buscapé
</commit_message>
<xml_diff>
--- a/buscas.xlsx
+++ b/buscas.xlsx
@@ -43,7 +43,25 @@
     <t xml:space="preserve">rtx 3060</t>
   </si>
   <si>
-    <t xml:space="preserve">zota galax</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">zota galax </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">usado seminovo</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -53,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -83,6 +101,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,10 +180,10 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.68"/>
@@ -192,10 +216,10 @@
         <v>3000</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>3500</v>
+        <v>3800</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Crie um laço de repetição fazer as buscas para cada produto da tabela de produtos
</commit_message>
<xml_diff>
--- a/buscas.xlsx
+++ b/buscas.xlsx
@@ -43,25 +43,7 @@
     <t xml:space="preserve">rtx 3060</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">zota galax </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">usado seminovo</t>
-    </r>
+    <t xml:space="preserve">zota galax usado seminovo</t>
   </si>
 </sst>
 </file>
@@ -71,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -101,12 +83,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -180,7 +156,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -227,7 +203,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>4000</v>
+        <v>2300</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>4500</v>

</xml_diff>